<commit_message>
add new project products.py
</commit_message>
<xml_diff>
--- a/MontysOdds.xlsx
+++ b/MontysOdds.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="80">
   <si>
     <t>n</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>3/20</t>
+  </si>
+  <si>
+    <t>(n+m)/(n-m)n</t>
   </si>
 </sst>
 </file>
@@ -587,13 +590,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -608,6 +614,12 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>